<commit_message>
Add Export Notes UI for AB#12143.
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/NotesReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/NotesReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_bugs\Apps\WebClient\src\Server\Assets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianjang/Repo/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D7D065-5CEA-48C8-9B38-A077EC6C95D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCDB919-0CD0-DE4E-A0BD-32787C3606C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="-42720" yWindow="920" windowWidth="34560" windowHeight="21580" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,10 @@
     <t>{d.records[i+1].title}</t>
   </si>
   <si>
-    <t>{d.records[i].notes}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].notes}</t>
+    <t>{d.records[i+1].note}</t>
+  </si>
+  <si>
+    <t>{d.records[i].note}</t>
   </si>
 </sst>
 </file>
@@ -437,16 +437,16 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.296875" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -465,10 +465,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -476,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Export Notes UI for AB#12143. (#3200)
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/NotesReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/NotesReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_bugs\Apps\WebClient\src\Server\Assets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianjang/Repo/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D7D065-5CEA-48C8-9B38-A077EC6C95D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCDB919-0CD0-DE4E-A0BD-32787C3606C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
+    <workbookView xWindow="-42720" yWindow="920" windowWidth="34560" windowHeight="21580" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,10 @@
     <t>{d.records[i+1].title}</t>
   </si>
   <si>
-    <t>{d.records[i].notes}</t>
-  </si>
-  <si>
-    <t>{d.records[i+1].notes}</t>
+    <t>{d.records[i+1].note}</t>
+  </si>
+  <si>
+    <t>{d.records[i].note}</t>
   </si>
 </sst>
 </file>
@@ -437,16 +437,16 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.296875" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -465,10 +465,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -476,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>